<commit_message>
Remove EducationLevelType and OccupationType, add Person.EducationLevel and Person.Occupation varchar columns.
</commit_message>
<xml_diff>
--- a/adapters/custody-analytics-staging-adapter/src/test/resources/codeSpreadSheets/PimaCountyAnalyticsCodeTables.xlsx
+++ b/adapters/custody-analytics-staging-adapter/src/test/resources/codeSpreadSheets/PimaCountyAnalyticsCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="700" windowWidth="25620" windowHeight="16060" tabRatio="951" firstSheet="4" activeTab="13"/>
+    <workbookView xWindow="3140" yWindow="700" windowWidth="25620" windowHeight="16060" tabRatio="951" firstSheet="7" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Facility" sheetId="9" r:id="rId1"/>
@@ -16,20 +16,18 @@
     <sheet name="CaseStatusType" sheetId="3" r:id="rId7"/>
     <sheet name="ChargeClassType" sheetId="31" r:id="rId8"/>
     <sheet name="DomicileStatusType" sheetId="23" r:id="rId9"/>
-    <sheet name="EducationLevelType" sheetId="13" r:id="rId10"/>
-    <sheet name="JurisdictionType" sheetId="2" r:id="rId11"/>
-    <sheet name="LanguageType" sheetId="15" r:id="rId12"/>
-    <sheet name="MedicaidStatusType" sheetId="33" r:id="rId13"/>
-    <sheet name="MilitaryServiceStatusType" sheetId="16" r:id="rId14"/>
-    <sheet name="OccupationType" sheetId="12" r:id="rId15"/>
-    <sheet name="PersonEthnicityType" sheetId="17" r:id="rId16"/>
-    <sheet name="PersonRaceType" sheetId="7" r:id="rId17"/>
-    <sheet name="PersonSexType" sheetId="6" r:id="rId18"/>
-    <sheet name="ProgramEligibilityType" sheetId="22" r:id="rId19"/>
-    <sheet name="SexOffenderStatusType" sheetId="25" r:id="rId20"/>
-    <sheet name="TreatmentAdmissionReasonType" sheetId="28" r:id="rId21"/>
-    <sheet name="TreatmentStatusType" sheetId="27" r:id="rId22"/>
-    <sheet name="WorkReleaseStatusType" sheetId="24" r:id="rId23"/>
+    <sheet name="JurisdictionType" sheetId="2" r:id="rId10"/>
+    <sheet name="LanguageType" sheetId="15" r:id="rId11"/>
+    <sheet name="MedicaidStatusType" sheetId="33" r:id="rId12"/>
+    <sheet name="MilitaryServiceStatusType" sheetId="16" r:id="rId13"/>
+    <sheet name="PersonEthnicityType" sheetId="17" r:id="rId14"/>
+    <sheet name="PersonRaceType" sheetId="7" r:id="rId15"/>
+    <sheet name="PersonSexType" sheetId="6" r:id="rId16"/>
+    <sheet name="ProgramEligibilityType" sheetId="22" r:id="rId17"/>
+    <sheet name="SexOffenderStatusType" sheetId="25" r:id="rId18"/>
+    <sheet name="TreatmentAdmissionReasonType" sheetId="28" r:id="rId19"/>
+    <sheet name="TreatmentStatusType" sheetId="27" r:id="rId20"/>
+    <sheet name="WorkReleaseStatusType" sheetId="24" r:id="rId21"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="429">
   <si>
     <t>JurisdictionTypeID</t>
   </si>
@@ -68,18 +66,6 @@
   </si>
   <si>
     <t>Capacity</t>
-  </si>
-  <si>
-    <t>OccupationTypeID</t>
-  </si>
-  <si>
-    <t>OccupationTypeDescription</t>
-  </si>
-  <si>
-    <t>EducationLevelTypeID</t>
-  </si>
-  <si>
-    <t>EducationLevelTypeDescription</t>
   </si>
   <si>
     <t>LanguageTypeID</t>
@@ -1906,7 +1892,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1932,13 +1918,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C2">
         <v>2474</v>
       </c>
       <c r="D2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1946,10 +1932,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1964,49 +1950,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="5" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -2033,10 +1976,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2044,10 +1987,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2055,10 +1998,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2066,10 +2009,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2077,10 +2020,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C6" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2088,10 +2031,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C7" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2099,10 +2042,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C8" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2110,10 +2053,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C9" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2121,10 +2064,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C10" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2132,10 +2075,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C11" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2143,10 +2086,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C12" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2154,10 +2097,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2165,10 +2108,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2176,10 +2119,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2187,10 +2130,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C16" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2198,10 +2141,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C17" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2209,10 +2152,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C18" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2220,10 +2163,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C19" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2231,10 +2174,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2248,7 +2191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C47"/>
   <sheetViews>
@@ -2264,10 +2207,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2275,10 +2218,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2286,10 +2229,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2297,10 +2240,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2308,10 +2251,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2319,10 +2262,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2330,10 +2273,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2341,10 +2284,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2352,10 +2295,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2363,10 +2306,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C10" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2374,10 +2317,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2385,10 +2328,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2396,10 +2339,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2407,10 +2350,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C14" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2418,10 +2361,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2429,10 +2372,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C16" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2440,10 +2383,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C17" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2451,10 +2394,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C18" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2462,10 +2405,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C19" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2473,10 +2416,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C20" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2484,10 +2427,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C21" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2495,10 +2438,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C22" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2506,10 +2449,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C23" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2517,10 +2460,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C24" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2528,10 +2471,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C25" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2539,10 +2482,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C26" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2550,10 +2493,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C27" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2561,10 +2504,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C28" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2572,10 +2515,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C29" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2583,10 +2526,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C30" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2594,10 +2537,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C31" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2605,10 +2548,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C32" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2616,10 +2559,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C33" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2627,10 +2570,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C34" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2638,10 +2581,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C35" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2649,10 +2592,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C36" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2660,10 +2603,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C37" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2671,10 +2614,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C38" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2682,10 +2625,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C39" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2693,10 +2636,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C40" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2704,10 +2647,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C41" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2715,10 +2658,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C42" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2726,10 +2669,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C43" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2737,10 +2680,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C44" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2748,10 +2691,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C45" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2759,10 +2702,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C46" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2770,10 +2713,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2787,7 +2730,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2803,10 +2746,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2814,7 +2757,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2822,7 +2765,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2830,7 +2773,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2843,7 +2786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -2862,10 +2805,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2873,7 +2816,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2886,41 +2829,165 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="5" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.1640625" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>292</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>294</v>
+      </c>
+      <c r="C2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="31.5" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2939,9 +3006,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.5" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="3" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2957,10 +3023,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>298</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>298</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2968,10 +3034,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>299</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>299</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2979,10 +3045,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2998,91 +3064,49 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="31.5" customWidth="1"/>
-    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>310</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3098,57 +3122,35 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="5" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="2" max="3" width="28" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="B1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3172,17 +3174,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="37" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>312</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3190,7 +3191,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3198,7 +3199,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>328</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3206,7 +3207,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3236,10 +3237,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3247,10 +3248,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3258,10 +3259,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3269,10 +3270,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3280,10 +3281,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3291,10 +3292,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3302,10 +3303,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3313,10 +3314,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3324,10 +3325,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3335,10 +3336,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3346,10 +3347,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3357,10 +3358,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3368,10 +3369,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -3379,10 +3380,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -3390,10 +3391,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -3401,10 +3402,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3412,10 +3413,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -3423,10 +3424,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3434,10 +3435,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -3445,10 +3446,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -3456,10 +3457,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -3467,10 +3468,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -3478,10 +3479,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -3489,10 +3490,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -3500,10 +3501,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -3511,10 +3512,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -3522,10 +3523,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -3533,10 +3534,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -3544,10 +3545,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -3555,10 +3556,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -3566,10 +3567,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -3577,10 +3578,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -3588,10 +3589,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -3599,10 +3600,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C34" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -3610,10 +3611,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -3621,10 +3622,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -3632,10 +3633,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -3643,10 +3644,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -3654,10 +3655,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -3665,10 +3666,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C40" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -3676,10 +3677,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -3687,10 +3688,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -3698,10 +3699,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C43" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -3709,10 +3710,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C44" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -3720,10 +3721,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C45" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -3731,10 +3732,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C46" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -3742,10 +3743,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C47" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -3753,10 +3754,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C48" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -3764,10 +3765,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3782,107 +3783,6 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="5" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>312</v>
-      </c>
-      <c r="B1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>316</v>
-      </c>
-      <c r="B1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3899,10 +3799,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3910,7 +3810,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3918,7 +3818,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3926,7 +3826,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3940,7 +3840,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -3959,10 +3859,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3970,7 +3870,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -4001,10 +3901,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4012,7 +3912,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4020,7 +3920,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4028,7 +3928,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -4058,10 +3958,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4069,7 +3969,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4077,7 +3977,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4085,7 +3985,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4093,7 +3993,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4101,7 +4001,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4109,7 +4009,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4117,7 +4017,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4125,7 +4025,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4133,7 +4033,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4141,7 +4041,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4149,7 +4049,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4157,7 +4057,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4165,7 +4065,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4173,7 +4073,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4181,7 +4081,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -4189,7 +4089,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -4197,7 +4097,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -4205,7 +4105,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -4213,7 +4113,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4221,7 +4121,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4229,7 +4129,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -4237,7 +4137,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -4245,7 +4145,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4253,7 +4153,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4261,7 +4161,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4269,7 +4169,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -4277,7 +4177,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -4285,7 +4185,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -4293,7 +4193,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -4301,7 +4201,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -4309,7 +4209,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -4317,7 +4217,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4325,7 +4225,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -4333,7 +4233,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -4341,7 +4241,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -4349,7 +4249,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -4357,7 +4257,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -4365,7 +4265,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -4373,7 +4273,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -4381,7 +4281,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -4389,7 +4289,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -4397,7 +4297,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -4405,7 +4305,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -4413,7 +4313,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -4421,7 +4321,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -4429,7 +4329,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -4437,7 +4337,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -4445,7 +4345,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -4453,7 +4353,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -4461,7 +4361,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -4469,7 +4369,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -4477,7 +4377,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -4485,7 +4385,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -4493,7 +4393,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -4501,7 +4401,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -4509,7 +4409,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -4517,7 +4417,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -4525,7 +4425,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -4533,7 +4433,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -4541,7 +4441,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -4549,7 +4449,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -4557,7 +4457,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -4565,7 +4465,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -4573,7 +4473,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -4581,7 +4481,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -4589,7 +4489,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -4597,7 +4497,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -4605,7 +4505,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -4613,7 +4513,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -4621,7 +4521,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -4629,7 +4529,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -4637,7 +4537,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -4645,7 +4545,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -4653,7 +4553,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -4661,7 +4561,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -4669,7 +4569,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -4677,7 +4577,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -4685,7 +4585,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -4693,7 +4593,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -4701,7 +4601,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -4709,7 +4609,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -4717,7 +4617,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -4725,7 +4625,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -4733,7 +4633,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -4741,7 +4641,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -4749,7 +4649,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -4757,7 +4657,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -4765,7 +4665,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -4773,7 +4673,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -4781,7 +4681,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -4789,7 +4689,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -4797,7 +4697,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -4805,7 +4705,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -4813,7 +4713,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -4821,7 +4721,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -4829,7 +4729,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -4837,7 +4737,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -4845,7 +4745,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -4853,7 +4753,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -4861,7 +4761,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -4869,7 +4769,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -4877,7 +4777,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -4885,7 +4785,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -4893,7 +4793,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -4924,10 +4824,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4935,10 +4835,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -4946,10 +4846,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -4957,10 +4857,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -4968,10 +4868,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4979,10 +4879,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -4990,10 +4890,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -5037,7 +4937,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -5078,7 +4978,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -5108,10 +5008,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -5119,10 +5019,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -5130,10 +5030,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -5141,10 +5041,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -5152,10 +5052,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -5163,10 +5063,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C6" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -5174,10 +5074,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C7" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -5185,10 +5085,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C8" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -5196,10 +5096,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C9" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -5207,10 +5107,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C10" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -5218,10 +5118,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -5229,10 +5129,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -5240,10 +5140,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -5251,10 +5151,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -5262,10 +5162,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C15" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -5273,10 +5173,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C16" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -5284,10 +5184,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C17" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -5295,10 +5195,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C18" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -5306,10 +5206,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -5340,10 +5240,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5351,7 +5251,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5359,7 +5259,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5367,7 +5267,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add junit test for Pima county booking report processing.
</commit_message>
<xml_diff>
--- a/adapters/custody-analytics-staging-adapter/src/test/resources/codeSpreadSheets/PimaCountyAnalyticsCodeTables.xlsx
+++ b/adapters/custody-analytics-staging-adapter/src/test/resources/codeSpreadSheets/PimaCountyAnalyticsCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="700" windowWidth="25620" windowHeight="16060" tabRatio="951" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="3140" yWindow="700" windowWidth="25620" windowHeight="16060" tabRatio="951" firstSheet="8" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Facility" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="428">
   <si>
     <t>JurisdictionTypeID</t>
   </si>
@@ -977,15 +977,6 @@
     <t>Substance Abuse</t>
   </si>
   <si>
-    <t>TreatmentAdmissionTypeID</t>
-  </si>
-  <si>
-    <t>TreatmentAdmissionTypeDescription</t>
-  </si>
-  <si>
-    <t>Pima County Jail</t>
-  </si>
-  <si>
     <t>AgencyID</t>
   </si>
   <si>
@@ -995,9 +986,6 @@
     <t>SupervisionUnitTypeID</t>
   </si>
   <si>
-    <t>SupervisionUnitDescription</t>
-  </si>
-  <si>
     <t>Not Homeless</t>
   </si>
   <si>
@@ -1326,6 +1314,15 @@
   </si>
   <si>
     <t>VISITATION</t>
+  </si>
+  <si>
+    <t>SupervisionUnitTypeDescription</t>
+  </si>
+  <si>
+    <t>TreatmentAdmissionReasonTypeID</t>
+  </si>
+  <si>
+    <t>TreatmentAdmissionReasonTypeDescription</t>
   </si>
 </sst>
 </file>
@@ -1374,8 +1371,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1467,11 +1466,11 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1516,6 +1515,7 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1560,6 +1560,7 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1892,7 +1893,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1918,13 +1919,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C2">
         <v>2474</v>
       </c>
       <c r="D2" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2196,7 +2197,7 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2757,7 +2758,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2765,7 +2766,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2793,7 +2794,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2901,7 +2902,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2926,7 +2927,7 @@
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
     </row>
@@ -2937,7 +2938,7 @@
       <c r="B3" t="s">
         <v>121</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>2</v>
       </c>
     </row>
@@ -2948,7 +2949,7 @@
       <c r="B4" t="s">
         <v>122</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>3</v>
       </c>
     </row>
@@ -2959,7 +2960,7 @@
       <c r="B5" t="s">
         <v>123</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>4</v>
       </c>
     </row>
@@ -2970,7 +2971,7 @@
       <c r="B6" t="s">
         <v>124</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>5</v>
       </c>
     </row>
@@ -3066,7 +3067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3090,7 +3091,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3098,7 +3099,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3169,7 +3170,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3180,10 +3181,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>312</v>
+        <v>426</v>
       </c>
       <c r="B1" t="s">
-        <v>313</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3191,7 +3192,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3237,10 +3238,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3848,7 +3849,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3946,22 +3947,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
     <col min="3" max="3" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B1" t="s">
-        <v>318</v>
+        <v>425</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3969,7 +3971,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3977,7 +3979,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3985,7 +3987,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3993,7 +3995,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4001,7 +4003,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4009,7 +4011,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4017,7 +4019,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4025,7 +4027,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4033,7 +4035,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4049,7 +4051,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4057,7 +4059,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4065,7 +4067,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4073,7 +4075,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4081,7 +4083,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -4089,7 +4091,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -4097,7 +4099,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -4105,7 +4107,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -4113,7 +4115,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4121,7 +4123,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4129,7 +4131,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -4137,7 +4139,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -4145,7 +4147,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4153,7 +4155,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4161,7 +4163,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4169,7 +4171,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -4177,7 +4179,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -4185,7 +4187,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -4193,7 +4195,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -4201,7 +4203,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -4209,7 +4211,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -4217,7 +4219,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4225,7 +4227,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -4233,7 +4235,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -4241,7 +4243,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -4249,7 +4251,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -4257,7 +4259,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -4265,7 +4267,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -4273,7 +4275,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -4281,7 +4283,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -4289,7 +4291,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -4297,7 +4299,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -4305,7 +4307,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -4313,7 +4315,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -4321,7 +4323,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -4329,7 +4331,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -4337,7 +4339,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -4345,7 +4347,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -4353,7 +4355,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -4361,7 +4363,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -4369,7 +4371,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -4377,7 +4379,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -4385,7 +4387,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -4393,7 +4395,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -4401,7 +4403,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -4409,7 +4411,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -4417,7 +4419,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -4425,7 +4427,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -4433,7 +4435,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -4441,7 +4443,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -4449,7 +4451,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -4457,7 +4459,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -4465,7 +4467,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -4473,7 +4475,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -4481,7 +4483,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -4489,7 +4491,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -4497,7 +4499,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -4505,7 +4507,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -4513,7 +4515,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -4521,7 +4523,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -4529,7 +4531,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -4537,7 +4539,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -4545,7 +4547,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -4553,7 +4555,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -4561,7 +4563,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -4569,7 +4571,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -4577,7 +4579,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -4585,7 +4587,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -4593,7 +4595,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -4601,7 +4603,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -4609,7 +4611,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -4617,7 +4619,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -4625,7 +4627,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -4633,7 +4635,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -4641,7 +4643,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -4649,7 +4651,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -4657,7 +4659,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -4665,7 +4667,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -4673,7 +4675,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -4681,7 +4683,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -4689,7 +4691,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -4697,7 +4699,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -4705,7 +4707,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -4713,7 +4715,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -4721,7 +4723,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -4729,7 +4731,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -4737,7 +4739,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -4745,7 +4747,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -4753,7 +4755,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -4761,7 +4763,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -4769,7 +4771,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -4777,7 +4779,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -4785,7 +4787,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -5251,7 +5253,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5259,7 +5261,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>

<commit_message>
Reflect the latest DB changes:
1. Add ChargeDisposition to BookingCharge and CustodyStatusChangeCharge. 
2. Drop the CaseStatusType code table.
</commit_message>
<xml_diff>
--- a/adapters/custody-analytics-staging-adapter/src/test/resources/codeSpreadSheets/PimaCountyAnalyticsCodeTables.xlsx
+++ b/adapters/custody-analytics-staging-adapter/src/test/resources/codeSpreadSheets/PimaCountyAnalyticsCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="700" windowWidth="25620" windowHeight="16060" tabRatio="951" firstSheet="8" activeTab="16"/>
+    <workbookView xWindow="3140" yWindow="700" windowWidth="25620" windowHeight="16060" tabRatio="951" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Facility" sheetId="9" r:id="rId1"/>
@@ -13,21 +13,20 @@
     <sheet name="SupervisionUnitType" sheetId="10" r:id="rId4"/>
     <sheet name="BondStatusType" sheetId="18" r:id="rId5"/>
     <sheet name="BondType" sheetId="5" r:id="rId6"/>
-    <sheet name="CaseStatusType" sheetId="3" r:id="rId7"/>
-    <sheet name="ChargeClassType" sheetId="31" r:id="rId8"/>
-    <sheet name="DomicileStatusType" sheetId="23" r:id="rId9"/>
-    <sheet name="JurisdictionType" sheetId="2" r:id="rId10"/>
-    <sheet name="LanguageType" sheetId="15" r:id="rId11"/>
-    <sheet name="MedicaidStatusType" sheetId="33" r:id="rId12"/>
-    <sheet name="MilitaryServiceStatusType" sheetId="16" r:id="rId13"/>
-    <sheet name="PersonEthnicityType" sheetId="17" r:id="rId14"/>
-    <sheet name="PersonRaceType" sheetId="7" r:id="rId15"/>
-    <sheet name="PersonSexType" sheetId="6" r:id="rId16"/>
-    <sheet name="ProgramEligibilityType" sheetId="22" r:id="rId17"/>
-    <sheet name="SexOffenderStatusType" sheetId="25" r:id="rId18"/>
-    <sheet name="TreatmentAdmissionReasonType" sheetId="28" r:id="rId19"/>
-    <sheet name="TreatmentStatusType" sheetId="27" r:id="rId20"/>
-    <sheet name="WorkReleaseStatusType" sheetId="24" r:id="rId21"/>
+    <sheet name="ChargeClassType" sheetId="31" r:id="rId7"/>
+    <sheet name="DomicileStatusType" sheetId="23" r:id="rId8"/>
+    <sheet name="JurisdictionType" sheetId="2" r:id="rId9"/>
+    <sheet name="LanguageType" sheetId="15" r:id="rId10"/>
+    <sheet name="MedicaidStatusType" sheetId="33" r:id="rId11"/>
+    <sheet name="MilitaryServiceStatusType" sheetId="16" r:id="rId12"/>
+    <sheet name="PersonEthnicityType" sheetId="17" r:id="rId13"/>
+    <sheet name="PersonRaceType" sheetId="7" r:id="rId14"/>
+    <sheet name="PersonSexType" sheetId="6" r:id="rId15"/>
+    <sheet name="ProgramEligibilityType" sheetId="22" r:id="rId16"/>
+    <sheet name="SexOffenderStatusType" sheetId="25" r:id="rId17"/>
+    <sheet name="TreatmentAdmissionReasonType" sheetId="28" r:id="rId18"/>
+    <sheet name="TreatmentStatusType" sheetId="27" r:id="rId19"/>
+    <sheet name="WorkReleaseStatusType" sheetId="24" r:id="rId20"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -39,18 +38,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="426">
   <si>
     <t>JurisdictionTypeID</t>
   </si>
   <si>
     <t>JurisdictionTypeDescription</t>
-  </si>
-  <si>
-    <t>CaseStatusTypeID</t>
-  </si>
-  <si>
-    <t>CaseStatusTypeDescription</t>
   </si>
   <si>
     <t>BondTypeID</t>
@@ -1905,13 +1898,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1919,13 +1912,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C2">
         <v>2474</v>
       </c>
       <c r="D2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1933,10 +1926,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1951,248 +1944,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="34.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>258</v>
-      </c>
-      <c r="C3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>260</v>
-      </c>
-      <c r="C4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>262</v>
-      </c>
-      <c r="C5" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>264</v>
-      </c>
-      <c r="C6" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>266</v>
-      </c>
-      <c r="C7" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C8" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>270</v>
-      </c>
-      <c r="C9" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>272</v>
-      </c>
-      <c r="C10" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>274</v>
-      </c>
-      <c r="C11" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>276</v>
-      </c>
-      <c r="C12" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>277</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>278</v>
-      </c>
-      <c r="C14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>279</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>281</v>
-      </c>
-      <c r="C16" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>283</v>
-      </c>
-      <c r="C17" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>285</v>
-      </c>
-      <c r="C18" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>287</v>
-      </c>
-      <c r="C19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C47"/>
   <sheetViews>
@@ -2208,10 +1959,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2219,10 +1970,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2230,10 +1981,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2241,10 +1992,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2252,10 +2003,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2263,10 +2014,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2274,10 +2025,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2285,10 +2036,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2296,10 +2047,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2307,10 +2058,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2318,10 +2069,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2329,10 +2080,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2340,10 +2091,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2351,10 +2102,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2362,10 +2113,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2373,10 +2124,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2384,10 +2135,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2395,10 +2146,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2406,10 +2157,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2417,10 +2168,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2428,10 +2179,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2439,10 +2190,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2450,10 +2201,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2461,10 +2212,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2472,10 +2223,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2483,10 +2234,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2494,10 +2245,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2505,10 +2256,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C28" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2516,10 +2267,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C29" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2527,10 +2278,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2538,10 +2289,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C31" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2549,10 +2300,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C32" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2560,10 +2311,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2571,10 +2322,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C34" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2582,10 +2333,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2593,10 +2344,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C36" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2604,10 +2355,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C37" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2615,10 +2366,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C38" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2626,10 +2377,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C39" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2637,10 +2388,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C40" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2648,10 +2399,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C41" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2659,10 +2410,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C42" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2670,10 +2421,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C43" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2681,10 +2432,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C44" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2692,10 +2443,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C45" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2703,10 +2454,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C46" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2714,10 +2465,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2731,7 +2482,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2747,10 +2498,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2758,7 +2509,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2766,7 +2517,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2774,7 +2525,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2787,7 +2538,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -2806,10 +2557,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2817,7 +2568,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2830,7 +2581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -2847,10 +2598,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2858,10 +2609,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2869,10 +2620,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2880,10 +2631,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2897,7 +2648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2914,10 +2665,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2925,7 +2676,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -2936,7 +2687,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -2947,7 +2698,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -2958,7 +2709,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -2969,7 +2720,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -2980,10 +2731,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2997,7 +2748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -3013,10 +2764,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3024,10 +2775,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3035,10 +2786,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3046,10 +2797,68 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3064,64 +2873,6 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="37" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -3140,10 +2891,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3151,7 +2902,64 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3170,21 +2978,22 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>426</v>
+        <v>288</v>
       </c>
       <c r="B1" t="s">
-        <v>427</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3192,7 +3001,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>321</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3200,7 +3009,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3208,7 +3017,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3238,10 +3047,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3249,10 +3058,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3260,10 +3069,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3271,10 +3080,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3282,10 +3091,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3293,10 +3102,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3304,10 +3113,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3315,10 +3124,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3326,10 +3135,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -3337,10 +3146,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -3348,10 +3157,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -3359,10 +3168,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -3370,10 +3179,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -3381,10 +3190,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -3392,10 +3201,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -3403,10 +3212,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3414,10 +3223,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -3425,10 +3234,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3436,10 +3245,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -3447,10 +3256,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -3458,10 +3267,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -3469,10 +3278,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -3480,10 +3289,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -3491,10 +3300,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -3502,10 +3311,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -3513,10 +3322,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -3524,10 +3333,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -3535,10 +3344,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -3546,10 +3355,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -3557,10 +3366,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -3568,10 +3377,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -3579,10 +3388,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -3590,10 +3399,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -3601,10 +3410,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -3612,10 +3421,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -3623,10 +3432,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C36" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -3634,10 +3443,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -3645,10 +3454,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -3656,10 +3465,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C39" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -3667,10 +3476,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -3678,10 +3487,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -3689,10 +3498,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -3700,10 +3509,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -3711,10 +3520,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -3722,10 +3531,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C45" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -3733,10 +3542,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C46" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -3744,10 +3553,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C47" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -3755,10 +3564,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C48" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -3766,10 +3575,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3784,64 +3593,6 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>290</v>
-      </c>
-      <c r="B1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -3860,10 +3611,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3871,7 +3622,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3902,10 +3653,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3913,7 +3664,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3921,7 +3672,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3929,7 +3680,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -3960,10 +3711,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3971,7 +3722,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3979,7 +3730,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3987,7 +3738,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3995,7 +3746,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4003,7 +3754,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4011,7 +3762,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4019,7 +3770,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4027,7 +3778,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4035,7 +3786,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4043,7 +3794,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4051,7 +3802,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4059,7 +3810,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4067,7 +3818,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4075,7 +3826,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4083,7 +3834,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -4091,7 +3842,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -4099,7 +3850,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -4107,7 +3858,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -4115,7 +3866,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4123,7 +3874,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4131,7 +3882,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -4139,7 +3890,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -4147,7 +3898,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4155,7 +3906,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4163,7 +3914,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4171,7 +3922,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -4179,7 +3930,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -4187,7 +3938,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -4195,7 +3946,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -4203,7 +3954,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -4211,7 +3962,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -4219,7 +3970,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4227,7 +3978,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -4235,7 +3986,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -4243,7 +3994,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -4251,7 +4002,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -4259,7 +4010,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -4267,7 +4018,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -4275,7 +4026,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -4283,7 +4034,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -4291,7 +4042,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -4299,7 +4050,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -4307,7 +4058,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -4315,7 +4066,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -4323,7 +4074,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -4331,7 +4082,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -4339,7 +4090,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -4347,7 +4098,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -4355,7 +4106,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -4363,7 +4114,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -4371,7 +4122,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -4379,7 +4130,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -4387,7 +4138,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -4395,7 +4146,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -4403,7 +4154,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -4411,7 +4162,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -4419,7 +4170,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -4427,7 +4178,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -4435,7 +4186,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -4443,7 +4194,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -4451,7 +4202,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -4459,7 +4210,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -4467,7 +4218,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -4475,7 +4226,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -4483,7 +4234,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -4491,7 +4242,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -4499,7 +4250,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -4507,7 +4258,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -4515,7 +4266,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -4523,7 +4274,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -4531,7 +4282,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -4539,7 +4290,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -4547,7 +4298,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -4555,7 +4306,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -4563,7 +4314,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -4571,7 +4322,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -4579,7 +4330,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -4587,7 +4338,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -4595,7 +4346,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -4603,7 +4354,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -4611,7 +4362,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -4619,7 +4370,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -4627,7 +4378,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -4635,7 +4386,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -4643,7 +4394,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -4651,7 +4402,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -4659,7 +4410,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -4667,7 +4418,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -4675,7 +4426,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -4683,7 +4434,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -4691,7 +4442,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -4699,7 +4450,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -4707,7 +4458,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -4715,7 +4466,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -4723,7 +4474,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -4731,7 +4482,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -4739,7 +4490,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -4747,7 +4498,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -4755,7 +4506,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -4763,7 +4514,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -4771,7 +4522,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -4779,7 +4530,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -4787,7 +4538,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -4795,7 +4546,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4826,10 +4577,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4837,10 +4588,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -4848,10 +4599,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -4859,10 +4610,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -4870,10 +4621,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4881,10 +4632,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -4892,10 +4643,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4928,10 +4679,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4939,7 +4690,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4954,33 +4705,222 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" customWidth="1"/>
-    <col min="3" max="3" width="28.5" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>220</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>241</v>
+      </c>
+      <c r="C11" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>242</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
         <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>243</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>244</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>246</v>
+      </c>
+      <c r="C15" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>248</v>
+      </c>
+      <c r="C16" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>250</v>
+      </c>
+      <c r="C17" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>252</v>
+      </c>
+      <c r="C18" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4995,237 +4935,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>229</v>
-      </c>
-      <c r="C4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>231</v>
-      </c>
-      <c r="C5" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>233</v>
-      </c>
-      <c r="C6" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>235</v>
-      </c>
-      <c r="C7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>237</v>
-      </c>
-      <c r="C8" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>239</v>
-      </c>
-      <c r="C9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>241</v>
-      </c>
-      <c r="C10" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>243</v>
-      </c>
-      <c r="C11" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>244</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>245</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>246</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>248</v>
-      </c>
-      <c r="C15" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>250</v>
-      </c>
-      <c r="C16" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>252</v>
-      </c>
-      <c r="C17" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>254</v>
-      </c>
-      <c r="C18" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -5242,10 +4951,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5253,7 +4962,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5261,7 +4970,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5269,7 +4978,249 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>262</v>
+      </c>
+      <c r="C6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>264</v>
+      </c>
+      <c r="C7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C9" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>270</v>
+      </c>
+      <c r="C10" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C12" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
         <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>276</v>
+      </c>
+      <c r="C14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>277</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>279</v>
+      </c>
+      <c r="C16" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>281</v>
+      </c>
+      <c r="C17" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>283</v>
+      </c>
+      <c r="C18" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the Pima code spreadsheet to the latest.
</commit_message>
<xml_diff>
--- a/adapters/custody-analytics-staging-adapter/src/test/resources/codeSpreadSheets/PimaCountyAnalyticsCodeTables.xlsx
+++ b/adapters/custody-analytics-staging-adapter/src/test/resources/codeSpreadSheets/PimaCountyAnalyticsCodeTables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="2360" windowWidth="25440" windowHeight="12240" tabRatio="951"/>
+    <workbookView xWindow="5700" yWindow="2820" windowWidth="25440" windowHeight="12240" tabRatio="951" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Facility" sheetId="9" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="PersonRaceType" sheetId="7" r:id="rId13"/>
     <sheet name="PersonSexType" sheetId="6" r:id="rId14"/>
     <sheet name="ProgramEligibilityType" sheetId="22" r:id="rId15"/>
+    <sheet name="TreatmentAdmissionReasonType" sheetId="34" r:id="rId16"/>
+    <sheet name="TreatmentStatusType" sheetId="35" r:id="rId17"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="436">
   <si>
     <t>JurisdictionTypeID</t>
   </si>
@@ -146,15 +148,9 @@
     <t>EMS</t>
   </si>
   <si>
-    <t>EMS: Pima Co. Sheriff's Dept.</t>
-  </si>
-  <si>
     <t>Fed Bureau of Investigation</t>
   </si>
   <si>
-    <t>FIRE: Pima Co. Sheriff's Dept.</t>
-  </si>
-  <si>
     <t>INS</t>
   </si>
   <si>
@@ -206,15 +202,9 @@
     <t>PCSD</t>
   </si>
   <si>
-    <t>Pima County Sheriff's Dept.</t>
-  </si>
-  <si>
     <t>PINL</t>
   </si>
   <si>
-    <t>Pinal County Sheriff's Dept</t>
-  </si>
-  <si>
     <t>UPRR</t>
   </si>
   <si>
@@ -284,9 +274,6 @@
     <t>NSIS</t>
   </si>
   <si>
-    <t>NSIS: Pima Co. Sheriff's Dept.</t>
-  </si>
-  <si>
     <t>PAC</t>
   </si>
   <si>
@@ -311,15 +298,9 @@
     <t>MAPO</t>
   </si>
   <si>
-    <t>Marana Prosecutor's Office</t>
-  </si>
-  <si>
     <t>SPO</t>
   </si>
   <si>
-    <t>Sahuarita Prosecutor's Office</t>
-  </si>
-  <si>
     <t>AAG</t>
   </si>
   <si>
@@ -647,9 +628,6 @@
     <t>TOHO</t>
   </si>
   <si>
-    <t>Tohono O'Odham Speaker</t>
-  </si>
-  <si>
     <t>TONG</t>
   </si>
   <si>
@@ -1305,6 +1283,66 @@
   </si>
   <si>
     <t>X_Code</t>
+  </si>
+  <si>
+    <t>TreatmentAdmissionReasonTypeID</t>
+  </si>
+  <si>
+    <t>TreatmentAdmissionReasonTypeDescription</t>
+  </si>
+  <si>
+    <t>Court-Ordered Treatment</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Danger To Self</t>
+  </si>
+  <si>
+    <t>Danger To Others</t>
+  </si>
+  <si>
+    <t>Gravely Disabled</t>
+  </si>
+  <si>
+    <t>Persistently and Acutely Disabled</t>
+  </si>
+  <si>
+    <t>TreatmentStatusTypeID</t>
+  </si>
+  <si>
+    <t>TreatmentStatusTypeDescription</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>EMS: Pima Co. Sheriff Dept.</t>
+  </si>
+  <si>
+    <t>FIRE: Pima Co. Sheriff Dept.</t>
+  </si>
+  <si>
+    <t>Pima County Sheriff Dept.</t>
+  </si>
+  <si>
+    <t>Pinal County Sheriff Dept</t>
+  </si>
+  <si>
+    <t>NSIS: Pima Co. Sheriff Dept.</t>
+  </si>
+  <si>
+    <t>Marana Prosecutor Office</t>
+  </si>
+  <si>
+    <t>Sahuarita Prosecutor Office</t>
+  </si>
+  <si>
+    <t>Tohono O\'Odham Speaker</t>
   </si>
 </sst>
 </file>
@@ -1353,10 +1391,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="137">
+  <cellStyleXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1498,7 +1534,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="137">
+  <cellStyles count="135">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1566,7 +1602,6 @@
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1634,7 +1669,6 @@
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1969,20 +2003,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="42.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.875" customWidth="1"/>
+    <col min="3" max="3" width="20.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1993,29 +2026,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C2">
         <v>2474</v>
-      </c>
-      <c r="D2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2034,16 +2053,16 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.625" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -2051,505 +2070,505 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C14" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C17" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C18" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C20" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C21" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C22" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C23" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C24" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C25" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C26" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C27" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C28" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C29" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C30" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C31" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C32" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C33" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C34" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C35" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C36" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C37" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C38" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>204</v>
+        <v>435</v>
       </c>
       <c r="C39" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C40" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C41" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C42" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C43" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C44" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C45" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="C46" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2579,37 +2598,37 @@
       <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2636,37 +2655,37 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.625" customWidth="1"/>
     <col min="2" max="2" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2693,25 +2712,25 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="31.5" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B1" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2722,51 +2741,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2796,24 +2815,24 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.125" customWidth="1"/>
     <col min="2" max="3" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B1" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2824,7 +2843,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2835,7 +2854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2861,18 +2880,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="BI1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.625" customWidth="1"/>
     <col min="2" max="2" width="37" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2880,23 +2899,23 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2915,32 +2934,118 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.125" customWidth="1"/>
+    <col min="2" max="2" width="31.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>419</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.125" customWidth="1"/>
+    <col min="2" max="2" width="28.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B1" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="C1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2951,7 +3056,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2962,7 +3067,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2973,7 +3078,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2984,480 +3089,480 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>428</v>
       </c>
       <c r="C6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>429</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>430</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>431</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>432</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>433</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>434</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C37" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C40" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C42" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C44" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C45" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C46" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C47" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C48" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3481,49 +3586,73 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>299</v>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -3541,105 +3670,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B105"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection sqref="A1:B105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.1640625" customWidth="1"/>
+    <col min="2" max="2" width="34.25" customWidth="1"/>
     <col min="3" max="3" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3647,743 +3776,743 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4412,48 +4541,48 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.875" customWidth="1"/>
+    <col min="2" max="2" width="27.375" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B1" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4464,29 +4593,29 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4516,16 +4645,16 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4533,10 +4662,10 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4547,59 +4676,59 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="C3" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="C4" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="C5" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="C6" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="C7" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -4621,211 +4750,211 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="C3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C6" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C10" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C11" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="C15" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C16" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C17" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C18" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4855,14 +4984,14 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -4870,23 +4999,23 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4913,13 +5042,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="34.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4927,208 +5056,208 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C3" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C5" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C6" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C7" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C9" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C10" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C11" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C12" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C16" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C17" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C18" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C19" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Fix the method of saving BHA method to save the BHACategories also.
</commit_message>
<xml_diff>
--- a/adapters/custody-analytics-staging-adapter/src/test/resources/codeSpreadSheets/PimaCountyAnalyticsCodeTables.xlsx
+++ b/adapters/custody-analytics-staging-adapter/src/test/resources/codeSpreadSheets/PimaCountyAnalyticsCodeTables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="2820" windowWidth="25440" windowHeight="12240" tabRatio="951" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="5700" yWindow="2820" windowWidth="25440" windowHeight="12240" tabRatio="951"/>
   </bookViews>
   <sheets>
     <sheet name="Facility" sheetId="9" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="436">
   <si>
     <t>JurisdictionTypeID</t>
   </si>
@@ -1391,8 +1391,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="135">
+  <cellStyleXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1534,7 +1536,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="135">
+  <cellStyles count="137">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1602,6 +1604,7 @@
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1669,6 +1672,7 @@
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2003,19 +2007,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="42.875" customWidth="1"/>
-    <col min="3" max="3" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="42.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2026,7 +2031,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2035,6 +2040,9 @@
       </c>
       <c r="C2">
         <v>2474</v>
+      </c>
+      <c r="D2" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -2056,13 +2064,13 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.625" customWidth="1"/>
-    <col min="2" max="2" width="24.375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -2073,7 +2081,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2084,7 +2092,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2095,7 +2103,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2106,7 +2114,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2117,7 +2125,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2128,7 +2136,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2139,7 +2147,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2150,7 +2158,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2161,7 +2169,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2172,7 +2180,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2183,7 +2191,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2194,7 +2202,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2205,7 +2213,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2216,7 +2224,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2227,7 +2235,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2238,7 +2246,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2249,7 +2257,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2260,7 +2268,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2271,7 +2279,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2282,7 +2290,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2293,7 +2301,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2304,7 +2312,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2315,7 +2323,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2326,7 +2334,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2337,7 +2345,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2348,7 +2356,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2359,7 +2367,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2370,7 +2378,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2381,7 +2389,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2392,7 +2400,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2403,7 +2411,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2414,7 +2422,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2425,7 +2433,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2436,7 +2444,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2447,7 +2455,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2458,7 +2466,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2469,7 +2477,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2480,7 +2488,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2491,7 +2499,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2502,7 +2510,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2513,7 +2521,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2524,7 +2532,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2535,7 +2543,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2546,7 +2554,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2557,7 +2565,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2568,7 +2576,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2598,13 +2606,13 @@
       <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>286</v>
       </c>
@@ -2612,7 +2620,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2620,7 +2628,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2628,7 +2636,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2655,13 +2663,13 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.625" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
     <col min="2" max="2" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>278</v>
       </c>
@@ -2669,7 +2677,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2677,7 +2685,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2685,7 +2693,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2712,14 +2720,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="31.5" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>288</v>
       </c>
@@ -2730,7 +2738,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2741,7 +2749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2752,7 +2760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2763,7 +2771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2774,7 +2782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2785,7 +2793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2815,13 +2823,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
     <col min="2" max="3" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>282</v>
       </c>
@@ -2832,7 +2840,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2843,7 +2851,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2854,7 +2862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2884,14 +2892,14 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
     <col min="2" max="2" width="37" customWidth="1"/>
-    <col min="3" max="3" width="30.375" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2899,7 +2907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2907,7 +2915,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2915,7 +2923,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2942,13 +2950,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="32.125" customWidth="1"/>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
     <col min="2" max="2" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>416</v>
       </c>
@@ -2956,7 +2964,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2964,7 +2972,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2974,6 +2982,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2985,13 +2998,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.125" customWidth="1"/>
-    <col min="2" max="2" width="28.875" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>424</v>
       </c>
@@ -2999,7 +3012,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3007,7 +3020,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3017,6 +3030,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3028,13 +3046,13 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="34.625" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>292</v>
       </c>
@@ -3045,7 +3063,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3056,7 +3074,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3067,7 +3085,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3078,7 +3096,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3089,7 +3107,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3100,7 +3118,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3111,7 +3129,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3122,7 +3140,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3133,7 +3151,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3144,7 +3162,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3155,7 +3173,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3166,7 +3184,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3177,7 +3195,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3188,7 +3206,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3199,7 +3217,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3210,7 +3228,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3221,7 +3239,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3232,7 +3250,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3243,7 +3261,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3254,7 +3272,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3265,7 +3283,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3276,7 +3294,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3287,7 +3305,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3298,7 +3316,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3309,7 +3327,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3320,7 +3338,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3331,7 +3349,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3342,7 +3360,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3353,7 +3371,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3364,7 +3382,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3375,7 +3393,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3386,7 +3404,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3397,7 +3415,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3408,7 +3426,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3419,7 +3437,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3430,7 +3448,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3441,7 +3459,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3452,7 +3470,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3463,7 +3481,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3474,7 +3492,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3485,7 +3503,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3496,7 +3514,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3507,7 +3525,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3518,7 +3536,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3529,7 +3547,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3540,7 +3558,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3551,7 +3569,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3562,7 +3580,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3588,18 +3606,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.375" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>284</v>
       </c>
@@ -3607,7 +3625,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3615,7 +3633,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3623,7 +3641,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3631,7 +3649,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3639,7 +3657,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3647,7 +3665,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3674,13 +3692,13 @@
       <selection sqref="A1:B105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="34.25" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
     <col min="3" max="3" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>294</v>
       </c>
@@ -3688,7 +3706,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3696,7 +3714,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3704,7 +3722,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3712,7 +3730,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3720,7 +3738,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3728,7 +3746,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3736,7 +3754,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3744,7 +3762,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3752,7 +3770,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3760,7 +3778,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3768,7 +3786,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3776,7 +3794,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3784,7 +3802,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3792,7 +3810,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3800,7 +3818,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3808,7 +3826,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3816,7 +3834,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3824,7 +3842,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3832,7 +3850,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3840,7 +3858,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3848,7 +3866,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3856,7 +3874,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3864,7 +3882,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3872,7 +3890,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3880,7 +3898,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3888,7 +3906,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3896,7 +3914,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3904,7 +3922,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3912,7 +3930,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3920,7 +3938,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3928,7 +3946,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3936,7 +3954,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3944,7 +3962,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3952,7 +3970,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3960,7 +3978,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3968,7 +3986,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3976,7 +3994,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3984,7 +4002,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3992,7 +4010,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4000,7 +4018,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4008,7 +4026,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4016,7 +4034,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4024,7 +4042,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4032,7 +4050,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4040,7 +4058,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4048,7 +4066,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4056,7 +4074,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4064,7 +4082,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4072,7 +4090,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4080,7 +4098,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4088,7 +4106,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4096,7 +4114,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4104,7 +4122,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4112,7 +4130,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4120,7 +4138,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4128,7 +4146,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4136,7 +4154,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4144,7 +4162,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4152,7 +4170,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4160,7 +4178,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4168,7 +4186,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4176,7 +4194,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4184,7 +4202,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4192,7 +4210,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4200,7 +4218,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4208,7 +4226,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4216,7 +4234,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4224,7 +4242,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4232,7 +4250,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4240,7 +4258,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4248,7 +4266,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4256,7 +4274,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4264,7 +4282,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4272,7 +4290,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4280,7 +4298,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4288,7 +4306,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4296,7 +4314,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4304,7 +4322,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4312,7 +4330,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4320,7 +4338,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4328,7 +4346,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4336,7 +4354,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4344,7 +4362,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4352,7 +4370,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4360,7 +4378,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4368,7 +4386,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4376,7 +4394,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4384,7 +4402,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4392,7 +4410,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4400,7 +4418,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4408,7 +4426,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4416,7 +4434,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4424,7 +4442,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4432,7 +4450,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4440,7 +4458,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4448,7 +4466,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4456,7 +4474,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4464,7 +4482,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4472,7 +4490,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4480,7 +4498,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4488,7 +4506,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4496,7 +4514,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4504,7 +4522,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4512,7 +4530,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4541,15 +4559,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.875" customWidth="1"/>
-    <col min="2" max="2" width="27.375" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="18.875" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>276</v>
       </c>
@@ -4560,7 +4578,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4571,7 +4589,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4582,7 +4600,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4593,7 +4611,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4604,7 +4622,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4615,7 +4633,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4648,13 +4666,13 @@
       <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="23.625" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4665,7 +4683,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4676,7 +4694,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4687,7 +4705,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4698,7 +4716,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4709,7 +4727,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4720,7 +4738,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4750,13 +4768,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>210</v>
       </c>
@@ -4767,7 +4785,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4778,7 +4796,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4789,7 +4807,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4800,7 +4818,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4811,7 +4829,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4822,7 +4840,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4833,7 +4851,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4844,7 +4862,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4855,7 +4873,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4866,7 +4884,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4877,7 +4895,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4888,7 +4906,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4899,7 +4917,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4910,7 +4928,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4921,7 +4939,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4932,7 +4950,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4943,7 +4961,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4954,7 +4972,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4984,14 +5002,14 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.875" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -4999,7 +5017,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5007,7 +5025,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5015,7 +5033,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5042,13 +5060,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="34.875" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5059,7 +5077,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5070,7 +5088,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5081,7 +5099,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5092,7 +5110,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5103,7 +5121,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5114,7 +5132,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5125,7 +5143,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5136,7 +5154,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5147,7 +5165,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5158,7 +5176,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5169,7 +5187,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5180,7 +5198,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5191,7 +5209,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5202,7 +5220,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5213,7 +5231,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5224,7 +5242,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5235,7 +5253,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5246,7 +5264,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5257,7 +5275,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Use the new element TreatmentStatusCode to retrieve the treatment status type from the reports.
</commit_message>
<xml_diff>
--- a/adapters/custody-analytics-staging-adapter/src/test/resources/codeSpreadSheets/PimaCountyAnalyticsCodeTables.xlsx
+++ b/adapters/custody-analytics-staging-adapter/src/test/resources/codeSpreadSheets/PimaCountyAnalyticsCodeTables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="2820" windowWidth="25440" windowHeight="12240" tabRatio="951"/>
+    <workbookView xWindow="600" yWindow="0" windowWidth="25440" windowHeight="12240" tabRatio="951" firstSheet="9" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Facility" sheetId="9" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="437">
   <si>
     <t>JurisdictionTypeID</t>
   </si>
@@ -1343,18 +1343,22 @@
   </si>
   <si>
     <t>Tohono O\'Odham Speaker</t>
+  </si>
+  <si>
+    <t>Crisis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1369,6 +1373,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1391,7 +1402,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="137">
+  <cellStyleXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1527,16 +1538,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="137">
+  <cellStyles count="135">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1604,7 +1614,6 @@
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1672,7 +1681,6 @@
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2009,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2041,7 +2049,7 @@
       <c r="C2">
         <v>2474</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>301</v>
       </c>
     </row>
@@ -2061,7 +2069,7 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2992,10 +3000,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3026,6 +3034,14 @@
       </c>
       <c r="B3" t="s">
         <v>427</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>436</v>
       </c>
     </row>
   </sheetData>

</xml_diff>